<commit_message>
V 2.0.2 se arreglo la fechar y hora de reimpresion
</commit_message>
<xml_diff>
--- a/reportes/10.10.2.246.xlsx
+++ b/reportes/10.10.2.246.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>HOSPITAL GENERAL SAN JUAN DE DIOS</t>
   </si>
@@ -31,10 +31,10 @@
     <t>No. Expediente Clínico</t>
   </si>
   <si>
-    <t>CALEL  ENRIQUE  ALEJANDRA  GUADALUPE</t>
-  </si>
-  <si>
-    <t>/201761938</t>
+    <t>CABRERA  AMBROSIO  KARLA  PAOLA</t>
+  </si>
+  <si>
+    <t>8327/201762643</t>
   </si>
   <si>
     <t>Fecha de Nacimiento ( Dia Mes Año)</t>
@@ -49,10 +49,10 @@
     <t>Sexo M  (   )   F  (    )</t>
   </si>
   <si>
-    <t>1998-02-24</t>
-  </si>
-  <si>
-    <t>19</t>
+    <t>1994-12-22</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
   <si>
     <t>GUATEMALA</t>
@@ -73,16 +73,13 @@
     <t>Documento de Identificación</t>
   </si>
   <si>
-    <t>CASADO</t>
-  </si>
-  <si>
-    <t>AMA DE CASA</t>
-  </si>
-  <si>
-    <t>GUATEMALTECA</t>
-  </si>
-  <si>
-    <t>NO PRESENTO</t>
+    <t>SOLTERO</t>
+  </si>
+  <si>
+    <t>RESCATISYA</t>
+  </si>
+  <si>
+    <t>SIN DOC</t>
   </si>
   <si>
     <t>En caso de emergencia notificar a:</t>
@@ -97,28 +94,28 @@
     <t>Teléfono</t>
   </si>
   <si>
-    <t>MANUEL MARROQUIN</t>
-  </si>
-  <si>
-    <t>ESPOSO</t>
-  </si>
-  <si>
-    <t>27 C. 7-08 Z. 3</t>
-  </si>
-  <si>
-    <t>5612-7683</t>
+    <t>GINA MORATAYA PAIZ</t>
+  </si>
+  <si>
+    <t>ENCARGADA</t>
+  </si>
+  <si>
+    <t>14 AV 2-50 Z.1</t>
+  </si>
+  <si>
+    <t>5605-2848</t>
   </si>
   <si>
     <t>Fecha de la asistencia Médica</t>
   </si>
   <si>
-    <t>Hora: 12:6:22</t>
-  </si>
-  <si>
-    <t>Area de urgencia: OBTESTRICIA</t>
-  </si>
-  <si>
-    <t>23/10/2017</t>
+    <t>Hora: 15:25:7</t>
+  </si>
+  <si>
+    <t>Area de urgencia: GINECOLOGIA</t>
+  </si>
+  <si>
+    <t>24/10/2017</t>
   </si>
   <si>
     <t>MEDICINA</t>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tipo de Consulta </t>
-  </si>
-  <si>
-    <t>urgencia</t>
   </si>
   <si>
     <t>URGENCIA</t>
@@ -1023,61 +1017,61 @@
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>25</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="17"/>
     </row>
     <row r="13" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>28</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>29</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="14"/>
     </row>
     <row r="14" ht="24" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>32</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>33</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -1085,35 +1079,33 @@
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="F15" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="G15" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="H15" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
-      <c r="D16" s="26" t="s">
-        <v>41</v>
-      </c>
+      <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
@@ -1122,11 +1114,11 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
@@ -1135,7 +1127,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
@@ -1147,7 +1139,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1169,7 +1161,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
@@ -1181,7 +1173,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1203,7 +1195,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
@@ -1215,7 +1207,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1309,13 +1301,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="F34" s="35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G34" s="35"/>
       <c r="H34" s="35"/>
@@ -1326,7 +1318,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1338,13 +1330,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B37" s="38"/>
       <c r="C37" s="38"/>
       <c r="D37" s="38"/>
       <c r="E37" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H37" s="34"/>
     </row>
@@ -1354,7 +1346,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B39" s="39"/>
       <c r="C39" s="39"/>
@@ -1424,7 +1416,7 @@
       <c r="C46" s="41"/>
       <c r="D46" s="41"/>
       <c r="E46" s="41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="41"/>

</xml_diff>